<commit_message>
succesfuly implented Gyroscopic Torque
</commit_message>
<xml_diff>
--- a/ThrustbenchTest.xlsx
+++ b/ThrustbenchTest.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MichaelGerits\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tud365-my.sharepoint.com/personal/mgerits_tudelft_nl/Documents/Documenten/MATLAB Drive/Digi_DART/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3ABE735-7499-4F05-9CB2-2B74413613E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4AB13914-3EC0-47EE-AA98-A3ACA4ED4DCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="24892" windowHeight="14914" xr2:uid="{B7ABD699-4E1A-4F9D-8BC7-D7094DF5DDE4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>RPM</t>
   </si>
@@ -62,9 +62,6 @@
     <t>K_f</t>
   </si>
   <si>
-    <t>corrected rpm Kf</t>
-  </si>
-  <si>
     <t>power(W)</t>
   </si>
   <si>
@@ -81,6 +78,18 @@
   </si>
   <si>
     <t>PWM</t>
+  </si>
+  <si>
+    <t>K_q</t>
+  </si>
+  <si>
+    <t>halved rpm K_q</t>
+  </si>
+  <si>
+    <t>halved rpm Kf</t>
+  </si>
+  <si>
+    <t>https://m-selig.ae.illinois.edu/props/propDB.html</t>
   </si>
 </sst>
 </file>
@@ -641,34 +650,34 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0873682028660428E-7</c:v>
+                  <c:v>9.1022330519130765E-6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.4176550673390447E-7</c:v>
+                  <c:v>3.6979677959958185E-5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.8003456316819478E-7</c:v>
+                  <c:v>4.0183136268041858E-5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.210094674153767E-7</c:v>
+                  <c:v>4.3613097956774634E-5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.5687844137292908E-7</c:v>
+                  <c:v>4.6615648145699593E-5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.6494517825779836E-7</c:v>
+                  <c:v>4.7290905329981897E-5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5.8261948966620265E-7</c:v>
+                  <c:v>4.8770401429346865E-5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>6.437231485267198E-7</c:v>
+                  <c:v>5.3885317810082142E-5</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>6.0587149789667293E-7</c:v>
+                  <c:v>5.0716800057529077E-5</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>6.0701424757203913E-7</c:v>
+                  <c:v>5.0812458306848541E-5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3438,10 +3447,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60AC58BE-9982-46A1-B8DA-A949D006F8AA}">
-  <dimension ref="B1:M20"/>
+  <dimension ref="B1:O20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D7" workbookViewId="0">
-      <selection activeCell="S14" sqref="S14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R19" sqref="R19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -3449,10 +3458,11 @@
     <col min="2" max="2" width="12.84375" customWidth="1"/>
     <col min="3" max="3" width="12.61328125" customWidth="1"/>
     <col min="4" max="4" width="19.3046875" customWidth="1"/>
-    <col min="10" max="10" width="11.84375" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="11.84375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:15" x14ac:dyDescent="0.4">
       <c r="B1" t="s">
         <v>3</v>
       </c>
@@ -3460,7 +3470,7 @@
         <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E1" t="s">
         <v>1</v>
@@ -3475,13 +3485,19 @@
         <v>7</v>
       </c>
       <c r="K1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" t="s">
         <v>8</v>
       </c>
-      <c r="M1" t="s">
-        <v>9</v>
+      <c r="N1" t="s">
+        <v>14</v>
+      </c>
+      <c r="O1" t="s">
+        <v>15</v>
       </c>
     </row>
-    <row r="2" spans="2:13" x14ac:dyDescent="0.4">
+    <row r="2" spans="2:15" x14ac:dyDescent="0.4">
       <c r="B2">
         <v>0</v>
       </c>
@@ -3513,8 +3529,16 @@
         <f>E2*F2</f>
         <v>0</v>
       </c>
+      <c r="N2" t="e">
+        <f t="shared" ref="N2:N12" si="0">M2/(C2^2*$B$20*$C$20^5) * 1/(2*PI())</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O2" t="e">
+        <f>M2*4/(C2^2*$B$20*$C$20^5) * 1/(2*PI())</f>
+        <v>#DIV/0!</v>
+      </c>
     </row>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:15" x14ac:dyDescent="0.4">
       <c r="B3">
         <v>4</v>
       </c>
@@ -3535,23 +3559,31 @@
         <v>-78</v>
       </c>
       <c r="I3">
-        <f t="shared" ref="I3:I12" si="0">B3*9.80665/1000</f>
+        <f t="shared" ref="I3:I12" si="1">B3*9.80665/1000</f>
         <v>3.92266E-2</v>
       </c>
       <c r="J3">
-        <f t="shared" ref="J3:J12" si="1">I3/(C3^2*$B$20*$C$20)</f>
-        <v>1.0873682028660428E-7</v>
+        <f>I3/(C3^2*$B$20*$C$20^4)</f>
+        <v>9.1022330519130765E-6</v>
       </c>
       <c r="K3">
-        <f t="shared" ref="K3:K12" si="2">I3*4/(C3^2*$B$20*$C$20)</f>
-        <v>4.3494728114641711E-7</v>
+        <f>I3*4/(C3^2*$B$20*$C$20^4)</f>
+        <v>3.6408932207652306E-5</v>
       </c>
       <c r="M3">
-        <f t="shared" ref="M3:M12" si="3">E3*F3</f>
+        <f t="shared" ref="M3:M12" si="2">E3*F3</f>
         <v>1.6275999999999999</v>
       </c>
+      <c r="N3">
+        <f t="shared" si="0"/>
+        <v>2.6294133934386181E-4</v>
+      </c>
+      <c r="O3">
+        <f t="shared" ref="O3:O12" si="3">M3*4/(C3^2*$B$20*$C$20^5) * 1/(2*PI())</f>
+        <v>1.0517653573754472E-3</v>
+      </c>
     </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.4">
+    <row r="4" spans="2:15" x14ac:dyDescent="0.4">
       <c r="B4">
         <v>74</v>
       </c>
@@ -3569,23 +3601,31 @@
         <v>0.59</v>
       </c>
       <c r="I4">
+        <f t="shared" si="1"/>
+        <v>0.72569209999999995</v>
+      </c>
+      <c r="J4">
+        <f t="shared" ref="J4:J12" si="5">I4/(C4^2*$B$20*$C$20^4)</f>
+        <v>3.6979677959958185E-5</v>
+      </c>
+      <c r="K4">
+        <f t="shared" ref="K4:K12" si="6">I4*4/(C4^2*$B$20*$C$20^4)</f>
+        <v>1.4791871183983274E-4</v>
+      </c>
+      <c r="M4">
+        <f t="shared" si="2"/>
+        <v>7.375</v>
+      </c>
+      <c r="N4">
         <f t="shared" si="0"/>
-        <v>0.72569209999999995</v>
-      </c>
-      <c r="J4">
-        <f t="shared" si="1"/>
-        <v>4.4176550673390447E-7</v>
-      </c>
-      <c r="K4">
-        <f t="shared" si="2"/>
-        <v>1.7670620269356179E-6</v>
-      </c>
-      <c r="M4">
+        <v>2.616475422930509E-4</v>
+      </c>
+      <c r="O4">
         <f t="shared" si="3"/>
-        <v>7.375</v>
+        <v>1.0465901691722036E-3</v>
       </c>
     </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:15" x14ac:dyDescent="0.4">
       <c r="B5">
         <v>194</v>
       </c>
@@ -3603,23 +3643,31 @@
         <v>1.52</v>
       </c>
       <c r="I5">
+        <f t="shared" si="1"/>
+        <v>1.9024901000000001</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="5"/>
+        <v>4.0183136268041858E-5</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="6"/>
+        <v>1.6073254507216743E-4</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="2"/>
+        <v>18.923999999999999</v>
+      </c>
+      <c r="N5">
         <f t="shared" si="0"/>
-        <v>1.9024901000000001</v>
-      </c>
-      <c r="J5">
-        <f t="shared" si="1"/>
-        <v>4.8003456316819478E-7</v>
-      </c>
-      <c r="K5">
-        <f t="shared" si="2"/>
-        <v>1.9201382526727791E-6</v>
-      </c>
-      <c r="M5">
+        <v>2.7827761310719371E-4</v>
+      </c>
+      <c r="O5">
         <f t="shared" si="3"/>
-        <v>18.923999999999999</v>
+        <v>1.1131104524287748E-3</v>
       </c>
     </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:15" x14ac:dyDescent="0.4">
       <c r="B6">
         <v>385</v>
       </c>
@@ -3637,23 +3685,31 @@
         <v>4.58</v>
       </c>
       <c r="I6">
+        <f t="shared" si="1"/>
+        <v>3.7755602499999998</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="5"/>
+        <v>4.3613097956774634E-5</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="6"/>
+        <v>1.7445239182709853E-4</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="2"/>
+        <v>56.608799999999995</v>
+      </c>
+      <c r="N6">
         <f t="shared" si="0"/>
-        <v>3.7755602499999998</v>
-      </c>
-      <c r="J6">
-        <f t="shared" si="1"/>
-        <v>5.210094674153767E-7</v>
-      </c>
-      <c r="K6">
-        <f t="shared" si="2"/>
-        <v>2.0840378696615068E-6</v>
-      </c>
-      <c r="M6">
+        <v>4.55264079992953E-4</v>
+      </c>
+      <c r="O6">
         <f t="shared" si="3"/>
-        <v>56.608799999999995</v>
+        <v>1.821056319971812E-3</v>
       </c>
     </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.4">
+    <row r="7" spans="2:15" x14ac:dyDescent="0.4">
       <c r="B7" s="1">
         <v>574</v>
       </c>
@@ -3673,23 +3729,31 @@
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1">
+        <f t="shared" si="1"/>
+        <v>5.6290171000000004</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="5"/>
+        <v>4.6615648145699593E-5</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="6"/>
+        <v>1.8646259258279837E-4</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="2"/>
+        <v>85.54</v>
+      </c>
+      <c r="N7">
         <f t="shared" si="0"/>
-        <v>5.6290171000000004</v>
-      </c>
-      <c r="J7" s="1">
-        <f t="shared" si="1"/>
-        <v>5.5687844137292908E-7</v>
-      </c>
-      <c r="K7">
-        <f t="shared" si="2"/>
-        <v>2.2275137654917163E-6</v>
-      </c>
-      <c r="M7">
+        <v>4.9318778372835464E-4</v>
+      </c>
+      <c r="O7">
         <f t="shared" si="3"/>
-        <v>85.54</v>
+        <v>1.9727511349134186E-3</v>
       </c>
     </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:15" x14ac:dyDescent="0.4">
       <c r="B8">
         <v>800</v>
       </c>
@@ -3707,23 +3771,31 @@
         <v>12.2</v>
       </c>
       <c r="I8">
+        <f t="shared" si="1"/>
+        <v>7.8453200000000001</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="5"/>
+        <v>4.7290905329981897E-5</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="6"/>
+        <v>1.8916362131992759E-4</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="2"/>
+        <v>145.54599999999999</v>
+      </c>
+      <c r="N8">
         <f t="shared" si="0"/>
-        <v>7.8453200000000001</v>
-      </c>
-      <c r="J8">
-        <f t="shared" si="1"/>
-        <v>5.6494517825779836E-7</v>
-      </c>
-      <c r="K8">
-        <f t="shared" si="2"/>
-        <v>2.2597807130311934E-6</v>
-      </c>
-      <c r="M8">
+        <v>6.108170420096934E-4</v>
+      </c>
+      <c r="O8">
         <f t="shared" si="3"/>
-        <v>145.54599999999999</v>
+        <v>2.4432681680387736E-3</v>
       </c>
     </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:15" x14ac:dyDescent="0.4">
       <c r="B9">
         <v>1020</v>
       </c>
@@ -3741,23 +3813,31 @@
         <v>18.510000000000002</v>
       </c>
       <c r="I9">
+        <f t="shared" si="1"/>
+        <v>10.002782999999999</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="5"/>
+        <v>4.8770401429346865E-5</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="6"/>
+        <v>1.9508160571738746E-4</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="2"/>
+        <v>215.64150000000004</v>
+      </c>
+      <c r="N9">
         <f t="shared" si="0"/>
-        <v>10.002782999999999</v>
-      </c>
-      <c r="J9">
-        <f t="shared" si="1"/>
-        <v>5.8261948966620265E-7</v>
-      </c>
-      <c r="K9">
-        <f t="shared" si="2"/>
-        <v>2.3304779586648106E-6</v>
-      </c>
-      <c r="M9">
+        <v>7.3200109824346656E-4</v>
+      </c>
+      <c r="O9">
         <f t="shared" si="3"/>
-        <v>215.64150000000004</v>
+        <v>2.9280043929738662E-3</v>
       </c>
     </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.4">
+    <row r="10" spans="2:15" x14ac:dyDescent="0.4">
       <c r="B10">
         <v>1236</v>
       </c>
@@ -3775,23 +3855,31 @@
         <v>25.5</v>
       </c>
       <c r="I10">
+        <f t="shared" si="1"/>
+        <v>12.1210194</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="5"/>
+        <v>5.3885317810082142E-5</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="6"/>
+        <v>2.1554127124032857E-4</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="2"/>
+        <v>290.19</v>
+      </c>
+      <c r="N10">
         <f t="shared" si="0"/>
-        <v>12.1210194</v>
-      </c>
-      <c r="J10">
-        <f t="shared" si="1"/>
-        <v>6.437231485267198E-7</v>
-      </c>
-      <c r="K10">
-        <f t="shared" si="2"/>
-        <v>2.5748925941068792E-6</v>
-      </c>
-      <c r="M10">
+        <v>8.9816814982650144E-4</v>
+      </c>
+      <c r="O10">
         <f t="shared" si="3"/>
-        <v>290.19</v>
+        <v>3.5926725993060057E-3</v>
       </c>
     </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.4">
+    <row r="11" spans="2:15" x14ac:dyDescent="0.4">
       <c r="B11">
         <v>1250</v>
       </c>
@@ -3809,23 +3897,31 @@
         <v>28.6</v>
       </c>
       <c r="I11">
+        <f t="shared" si="1"/>
+        <v>12.258312500000001</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="5"/>
+        <v>5.0716800057529077E-5</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="6"/>
+        <v>2.0286720023011631E-4</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="2"/>
+        <v>321.464</v>
+      </c>
+      <c r="N11">
         <f t="shared" si="0"/>
-        <v>12.258312500000001</v>
-      </c>
-      <c r="J11">
-        <f t="shared" si="1"/>
-        <v>6.0587149789667293E-7</v>
-      </c>
-      <c r="K11">
-        <f t="shared" si="2"/>
-        <v>2.4234859915866917E-6</v>
-      </c>
-      <c r="M11">
+        <v>9.2597104290832353E-4</v>
+      </c>
+      <c r="O11">
         <f t="shared" si="3"/>
-        <v>321.464</v>
+        <v>3.7038841716332941E-3</v>
       </c>
     </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.4">
+    <row r="12" spans="2:15" x14ac:dyDescent="0.4">
       <c r="B12">
         <v>1373</v>
       </c>
@@ -3843,46 +3939,67 @@
         <v>30</v>
       </c>
       <c r="I12">
+        <f t="shared" si="1"/>
+        <v>13.464530449999998</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="5"/>
+        <v>5.0812458306848541E-5</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="6"/>
+        <v>2.0324983322739416E-4</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="2"/>
+        <v>333</v>
+      </c>
+      <c r="N12">
         <f t="shared" si="0"/>
-        <v>13.464530449999998</v>
-      </c>
-      <c r="J12">
-        <f t="shared" si="1"/>
-        <v>6.0701424757203913E-7</v>
-      </c>
-      <c r="K12">
-        <f t="shared" si="2"/>
-        <v>2.4280569902881565E-6</v>
-      </c>
-      <c r="M12">
+        <v>8.749175595006934E-4</v>
+      </c>
+      <c r="O12">
         <f t="shared" si="3"/>
-        <v>333</v>
+        <v>3.4996702380027736E-3</v>
       </c>
     </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.4">
+    <row r="13" spans="2:15" x14ac:dyDescent="0.4">
       <c r="J13" s="2">
-        <f>SUM(J4:J12)</f>
-        <v>5.0038615406098386E-6</v>
+        <f>AVERAGE(J4:J12)</f>
+        <v>4.6540827029362526E-5</v>
       </c>
       <c r="K13" s="2">
-        <f>SUM(K4:K12)</f>
-        <v>2.0015446162439354E-5</v>
+        <f>AVERAGE(K4:K12)</f>
+        <v>1.8616330811745011E-4</v>
+      </c>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2">
+        <f t="shared" ref="L13:O13" si="7">AVERAGE(N4:N12)</f>
+        <v>6.1447243462335903E-4</v>
+      </c>
+      <c r="O13" s="2">
+        <f t="shared" si="7"/>
+        <v>2.4578897384934361E-3</v>
       </c>
     </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.4">
+    <row r="15" spans="2:15" x14ac:dyDescent="0.4">
       <c r="B15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" t="s">
         <v>10</v>
       </c>
-      <c r="C15" t="s">
+    </row>
+    <row r="16" spans="2:15" x14ac:dyDescent="0.4">
+      <c r="B16" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.4">
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>12</v>
       </c>
-      <c r="C16" t="s">
-        <v>13</v>
+      <c r="E16" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.4">

</xml_diff>